<commit_message>
add rate for RA
</commit_message>
<xml_diff>
--- a/inst/ext/IICT-Offer-CTUservices2024.xlsx
+++ b/inst/ext/IICT-Offer-CTUservices2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\CTUCosting\inst\ext\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0554FA7E-73BB-4CDD-8A8F-401A1B143B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B311CD7F-C91A-49A6-8947-788D6DE64610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5664" yWindow="12" windowWidth="17280" windowHeight="12168" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="330" yWindow="690" windowWidth="27900" windowHeight="16830" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -587,39 +587,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -632,8 +599,41 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -931,9 +931,9 @@
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1012,21 +1012,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.625" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="24.5703125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="49" style="7" customWidth="1"/>
-    <col min="2" max="2" width="14.75" style="7" customWidth="1"/>
-    <col min="3" max="3" width="19.25" style="7" customWidth="1"/>
-    <col min="4" max="8" width="8.375" style="7" customWidth="1"/>
-    <col min="9" max="9" width="16.25" style="7" customWidth="1"/>
-    <col min="10" max="10" width="17.75" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="7" customWidth="1"/>
+    <col min="4" max="8" width="8.42578125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
@@ -1095,10 +1095,10 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="31"/>
+      <c r="B13" s="27"/>
       <c r="C13" s="5"/>
       <c r="I13" s="5"/>
     </row>
@@ -1116,58 +1116,58 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26" t="s">
+      <c r="C16" s="25"/>
+      <c r="D16" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="H16" s="26" t="s">
+      <c r="H16" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="I16" s="26" t="s">
+      <c r="I16" s="25" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="26"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-    </row>
-    <row r="18" spans="1:9" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+    </row>
+    <row r="18" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
       <c r="B18" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-    </row>
-    <row r="19" spans="1:9" ht="12" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="s">
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="29" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="10"/>
@@ -1199,8 +1199,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
+    <row r="20" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="30"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12" t="s">
         <v>85</v>
@@ -1230,8 +1230,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A21" s="21" t="s">
+    <row r="21" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A21" s="31" t="s">
         <v>44</v>
       </c>
       <c r="B21" s="13" t="s">
@@ -1260,8 +1260,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
+    <row r="22" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="32"/>
       <c r="B22" s="15">
         <v>99</v>
       </c>
@@ -1294,7 +1294,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="22"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="13" t="s">
         <v>46</v>
       </c>
@@ -1321,8 +1321,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
+    <row r="24" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="33"/>
       <c r="B24" s="15">
         <v>99</v>
       </c>
@@ -1354,11 +1354,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="12.6" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="28" t="s">
+    <row r="25" spans="1:9" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="28"/>
+      <c r="B25" s="34"/>
       <c r="C25" s="10" t="s">
         <v>83</v>
       </c>
@@ -1387,9 +1387,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
-      <c r="B26" s="29"/>
+    <row r="26" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="30"/>
+      <c r="B26" s="30"/>
       <c r="C26" s="12" t="s">
         <v>85</v>
       </c>
@@ -1418,8 +1418,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A27" s="21" t="s">
+    <row r="27" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A27" s="31" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="13" t="s">
@@ -1448,10 +1448,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
+    <row r="28" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="32"/>
       <c r="B28" s="15">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>81</v>
@@ -1482,7 +1482,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="22"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="13" t="s">
         <v>46</v>
       </c>
@@ -1509,10 +1509,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
+    <row r="30" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="33"/>
       <c r="B30" s="15">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>81</v>
@@ -1542,8 +1542,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="12.6" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="28" t="s">
+    <row r="31" spans="1:9" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="34" t="s">
         <v>50</v>
       </c>
       <c r="B31" s="11"/>
@@ -1575,8 +1575,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
+    <row r="32" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="30"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12" t="s">
         <v>85</v>
@@ -1606,8 +1606,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A33" s="21" t="s">
+    <row r="33" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A33" s="31" t="s">
         <v>51</v>
       </c>
       <c r="B33" s="13" t="s">
@@ -1636,8 +1636,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
+    <row r="34" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="32"/>
       <c r="B34" s="15">
         <v>89</v>
       </c>
@@ -1669,8 +1669,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A35" s="22"/>
+    <row r="35" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A35" s="32"/>
       <c r="B35" s="13" t="s">
         <v>53</v>
       </c>
@@ -1697,8 +1697,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="23"/>
+    <row r="36" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="35"/>
       <c r="B36" s="15">
         <v>89</v>
       </c>
@@ -1730,8 +1730,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A37" s="21" t="s">
+    <row r="37" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A37" s="31" t="s">
         <v>54</v>
       </c>
       <c r="B37" s="13" t="s">
@@ -1760,8 +1760,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
+    <row r="38" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="32"/>
       <c r="B38" s="15">
         <v>89</v>
       </c>
@@ -1793,8 +1793,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A39" s="22"/>
+    <row r="39" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A39" s="32"/>
       <c r="B39" s="13" t="s">
         <v>53</v>
       </c>
@@ -1821,8 +1821,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23"/>
+    <row r="40" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="35"/>
       <c r="B40" s="15">
         <v>89</v>
       </c>
@@ -1854,8 +1854,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A41" s="21" t="s">
+    <row r="41" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A41" s="31" t="s">
         <v>55</v>
       </c>
       <c r="B41" s="13" t="s">
@@ -1884,8 +1884,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
+    <row r="42" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="32"/>
       <c r="B42" s="15">
         <v>89</v>
       </c>
@@ -1917,8 +1917,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A43" s="22"/>
+    <row r="43" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A43" s="32"/>
       <c r="B43" s="13" t="s">
         <v>53</v>
       </c>
@@ -1945,8 +1945,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
+    <row r="44" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="33"/>
       <c r="B44" s="15">
         <v>89</v>
       </c>
@@ -1978,8 +1978,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="12.6" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="28" t="s">
+    <row r="45" spans="1:9" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="34" t="s">
         <v>56</v>
       </c>
       <c r="B45" s="11"/>
@@ -2011,8 +2011,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
+    <row r="46" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="30"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12" t="s">
         <v>85</v>
@@ -2043,7 +2043,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="31" t="s">
         <v>57</v>
       </c>
       <c r="B47" s="13" t="s">
@@ -2072,8 +2072,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
+    <row r="48" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="32"/>
       <c r="B48" s="15">
         <v>81</v>
       </c>
@@ -2106,7 +2106,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="22"/>
+      <c r="A49" s="32"/>
       <c r="B49" s="13" t="s">
         <v>59</v>
       </c>
@@ -2133,8 +2133,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
+    <row r="50" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="35"/>
       <c r="B50" s="15">
         <v>81</v>
       </c>
@@ -2167,7 +2167,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="21" t="s">
+      <c r="A51" s="31" t="s">
         <v>60</v>
       </c>
       <c r="B51" s="13" t="s">
@@ -2196,8 +2196,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
+    <row r="52" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="32"/>
       <c r="B52" s="15">
         <v>81</v>
       </c>
@@ -2230,7 +2230,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A53" s="22"/>
+      <c r="A53" s="32"/>
       <c r="B53" s="13" t="s">
         <v>59</v>
       </c>
@@ -2257,8 +2257,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="24"/>
+    <row r="54" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="33"/>
       <c r="B54" s="15">
         <v>81</v>
       </c>
@@ -2290,8 +2290,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="12.6" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="28" t="s">
+    <row r="55" spans="1:9" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="34" t="s">
         <v>61</v>
       </c>
       <c r="B55" s="11"/>
@@ -2323,8 +2323,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="29"/>
+    <row r="56" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="30"/>
       <c r="B56" s="12"/>
       <c r="C56" s="12" t="s">
         <v>85</v>
@@ -2355,7 +2355,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A57" s="21" t="s">
+      <c r="A57" s="31" t="s">
         <v>57</v>
       </c>
       <c r="B57" s="13" t="s">
@@ -2384,8 +2384,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="22"/>
+    <row r="58" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="32"/>
       <c r="B58" s="15">
         <v>81</v>
       </c>
@@ -2417,8 +2417,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A59" s="22"/>
+    <row r="59" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A59" s="32"/>
       <c r="B59" s="13" t="s">
         <v>62</v>
       </c>
@@ -2445,8 +2445,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="23"/>
+    <row r="60" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="35"/>
       <c r="B60" s="15">
         <v>81</v>
       </c>
@@ -2479,7 +2479,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A61" s="21" t="s">
+      <c r="A61" s="31" t="s">
         <v>63</v>
       </c>
       <c r="B61" s="13" t="s">
@@ -2508,8 +2508,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="22"/>
+    <row r="62" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="32"/>
       <c r="B62" s="15">
         <v>81</v>
       </c>
@@ -2541,8 +2541,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A63" s="22"/>
+    <row r="63" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A63" s="32"/>
       <c r="B63" s="13" t="s">
         <v>62</v>
       </c>
@@ -2569,8 +2569,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="24"/>
+    <row r="64" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="33"/>
       <c r="B64" s="15">
         <v>81</v>
       </c>
@@ -2602,8 +2602,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="12.6" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="28" t="s">
+    <row r="65" spans="1:9" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="34" t="s">
         <v>64</v>
       </c>
       <c r="B65" s="11"/>
@@ -2635,8 +2635,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="29"/>
+    <row r="66" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="30"/>
       <c r="B66" s="12"/>
       <c r="C66" s="12" t="s">
         <v>85</v>
@@ -2667,7 +2667,7 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="21" t="s">
+      <c r="A67" s="31" t="s">
         <v>65</v>
       </c>
       <c r="B67" s="13" t="s">
@@ -2696,8 +2696,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="22"/>
+    <row r="68" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="32"/>
       <c r="B68" s="15">
         <v>89</v>
       </c>
@@ -2730,7 +2730,7 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A69" s="22"/>
+      <c r="A69" s="32"/>
       <c r="B69" s="13" t="s">
         <v>46</v>
       </c>
@@ -2757,8 +2757,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="23"/>
+    <row r="70" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="35"/>
       <c r="B70" s="15">
         <v>89</v>
       </c>
@@ -2791,7 +2791,7 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A71" s="21" t="s">
+      <c r="A71" s="31" t="s">
         <v>67</v>
       </c>
       <c r="B71" s="13" t="s">
@@ -2820,8 +2820,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="22"/>
+    <row r="72" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="32"/>
       <c r="B72" s="15">
         <v>89</v>
       </c>
@@ -2854,7 +2854,7 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A73" s="22"/>
+      <c r="A73" s="32"/>
       <c r="B73" s="13" t="s">
         <v>46</v>
       </c>
@@ -2881,8 +2881,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="24"/>
+    <row r="74" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="33"/>
       <c r="B74" s="15">
         <v>89</v>
       </c>
@@ -2914,8 +2914,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="12.6" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="28" t="s">
+    <row r="75" spans="1:9" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="34" t="s">
         <v>68</v>
       </c>
       <c r="B75" s="11"/>
@@ -2947,8 +2947,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="29"/>
+    <row r="76" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="30"/>
       <c r="B76" s="12"/>
       <c r="C76" s="12" t="s">
         <v>85</v>
@@ -2978,8 +2978,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A77" s="21" t="s">
+    <row r="77" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A77" s="31" t="s">
         <v>57</v>
       </c>
       <c r="B77" s="13" t="s">
@@ -3008,8 +3008,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="22"/>
+    <row r="78" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="32"/>
       <c r="B78" s="15">
         <v>0</v>
       </c>
@@ -3041,8 +3041,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A79" s="22"/>
+    <row r="79" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A79" s="32"/>
       <c r="B79" s="13" t="s">
         <v>62</v>
       </c>
@@ -3069,8 +3069,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="23"/>
+    <row r="80" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="35"/>
       <c r="B80" s="15">
         <v>0</v>
       </c>
@@ -3102,8 +3102,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A81" s="21" t="s">
+    <row r="81" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A81" s="31" t="s">
         <v>70</v>
       </c>
       <c r="B81" s="13" t="s">
@@ -3132,8 +3132,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="22"/>
+    <row r="82" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="32"/>
       <c r="B82" s="15">
         <v>0</v>
       </c>
@@ -3165,8 +3165,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A83" s="22"/>
+    <row r="83" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A83" s="32"/>
       <c r="B83" s="13" t="s">
         <v>62</v>
       </c>
@@ -3193,8 +3193,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="24"/>
+    <row r="84" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="33"/>
       <c r="B84" s="15">
         <v>0</v>
       </c>
@@ -3226,8 +3226,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="12.6" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="28" t="s">
+    <row r="85" spans="1:9" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="34" t="s">
         <v>71</v>
       </c>
       <c r="B85" s="11"/>
@@ -3259,8 +3259,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="29"/>
+    <row r="86" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="30"/>
       <c r="B86" s="12"/>
       <c r="C86" s="12" t="s">
         <v>85</v>
@@ -3290,8 +3290,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A87" s="21" t="s">
+    <row r="87" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A87" s="31" t="s">
         <v>72</v>
       </c>
       <c r="B87" s="13" t="s">
@@ -3320,8 +3320,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="22"/>
+    <row r="88" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="32"/>
       <c r="B88" s="15">
         <v>90</v>
       </c>
@@ -3354,7 +3354,7 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A89" s="22"/>
+      <c r="A89" s="32"/>
       <c r="B89" s="13" t="s">
         <v>46</v>
       </c>
@@ -3381,8 +3381,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="23"/>
+    <row r="90" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="35"/>
       <c r="B90" s="15">
         <v>90</v>
       </c>
@@ -3414,8 +3414,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A91" s="21" t="s">
+    <row r="91" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A91" s="31" t="s">
         <v>74</v>
       </c>
       <c r="B91" s="13" t="s">
@@ -3444,8 +3444,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="22"/>
+    <row r="92" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="32"/>
       <c r="B92" s="15">
         <v>90</v>
       </c>
@@ -3478,7 +3478,7 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A93" s="22"/>
+      <c r="A93" s="32"/>
       <c r="B93" s="13" t="s">
         <v>46</v>
       </c>
@@ -3505,8 +3505,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="23"/>
+    <row r="94" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="35"/>
       <c r="B94" s="15">
         <v>90</v>
       </c>
@@ -3538,8 +3538,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A95" s="21" t="s">
+    <row r="95" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A95" s="31" t="s">
         <v>75</v>
       </c>
       <c r="B95" s="13" t="s">
@@ -3568,8 +3568,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="22"/>
+    <row r="96" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="32"/>
       <c r="B96" s="15">
         <v>90</v>
       </c>
@@ -3602,7 +3602,7 @@
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A97" s="22"/>
+      <c r="A97" s="32"/>
       <c r="B97" s="13" t="s">
         <v>46</v>
       </c>
@@ -3629,8 +3629,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="24"/>
+    <row r="98" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="33"/>
       <c r="B98" s="15">
         <v>90</v>
       </c>
@@ -3662,8 +3662,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="12.6" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="28" t="s">
+    <row r="99" spans="1:9" ht="12.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="34" t="s">
         <v>76</v>
       </c>
       <c r="B99" s="11"/>
@@ -3695,8 +3695,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="12.6" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="29"/>
+    <row r="100" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="30"/>
       <c r="B100" s="12"/>
       <c r="C100" s="12" t="s">
         <v>85</v>
@@ -3726,8 +3726,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A101" s="21" t="s">
+    <row r="101" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A101" s="31" t="s">
         <v>77</v>
       </c>
       <c r="B101" s="13" t="s">
@@ -3756,8 +3756,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="22"/>
+    <row r="102" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="32"/>
       <c r="B102" s="15">
         <v>0</v>
       </c>
@@ -3790,7 +3790,7 @@
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A103" s="22"/>
+      <c r="A103" s="32"/>
       <c r="B103" s="13" t="s">
         <v>79</v>
       </c>
@@ -3817,8 +3817,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="23"/>
+    <row r="104" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A104" s="35"/>
       <c r="B104" s="15">
         <v>0</v>
       </c>
@@ -3850,8 +3850,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A105" s="21" t="s">
+    <row r="105" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A105" s="31" t="s">
         <v>80</v>
       </c>
       <c r="B105" s="13" t="s">
@@ -3880,8 +3880,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="22"/>
+    <row r="106" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="32"/>
       <c r="B106" s="15">
         <v>0</v>
       </c>
@@ -3914,7 +3914,7 @@
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A107" s="22"/>
+      <c r="A107" s="32"/>
       <c r="B107" s="13" t="s">
         <v>79</v>
       </c>
@@ -3941,8 +3941,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="23"/>
+    <row r="108" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="35"/>
       <c r="B108" s="15">
         <v>0</v>
       </c>
@@ -3974,8 +3974,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="22.8" x14ac:dyDescent="0.2">
-      <c r="A109" s="21" t="s">
+    <row r="109" spans="1:9" ht="24" x14ac:dyDescent="0.2">
+      <c r="A109" s="31" t="s">
         <v>55</v>
       </c>
       <c r="B109" s="13" t="s">
@@ -4004,8 +4004,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="22"/>
+    <row r="110" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="32"/>
       <c r="B110" s="15">
         <v>0</v>
       </c>
@@ -4038,7 +4038,7 @@
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A111" s="22"/>
+      <c r="A111" s="32"/>
       <c r="B111" s="13" t="s">
         <v>79</v>
       </c>
@@ -4065,8 +4065,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="24"/>
+    <row r="112" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="33"/>
       <c r="B112" s="15">
         <v>0</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="22.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="22.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A113" s="17" t="s">
         <v>91</v>
       </c>
@@ -4126,95 +4126,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="115" spans="1:9" ht="11.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="35" t="s">
+    <row r="114" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="1:9" ht="11.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="B115" s="35"/>
-      <c r="C115" s="35"/>
-      <c r="D115" s="32">
+      <c r="B115" s="24"/>
+      <c r="C115" s="24"/>
+      <c r="D115" s="21">
         <f>SUM(D113,D100,D86,D76,D66,D56,D46,D32,D26,D20)</f>
         <v>0</v>
       </c>
-      <c r="E115" s="32">
+      <c r="E115" s="21">
         <f t="shared" ref="E115:G115" si="56">SUM(E113,E100,E86,E76,E66,E56,E46,E32,E26,E20)</f>
         <v>0</v>
       </c>
-      <c r="F115" s="32">
+      <c r="F115" s="21">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="G115" s="32">
+      <c r="G115" s="21">
         <f t="shared" si="56"/>
         <v>0</v>
       </c>
-      <c r="H115" s="32">
+      <c r="H115" s="21">
         <f>SUM(D230,H100,H86,H76,H66,H56,H46,H32,H26,H20)</f>
         <v>0</v>
       </c>
-      <c r="I115" s="35">
+      <c r="I115" s="24">
         <f>SUM(I113,I100,I86,I76,I66,I56,I46,I32,I26,I20)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="26"/>
-      <c r="B116" s="26"/>
-      <c r="C116" s="26"/>
-      <c r="D116" s="33"/>
-      <c r="E116" s="33"/>
-      <c r="F116" s="33"/>
-      <c r="G116" s="33"/>
-      <c r="H116" s="33"/>
-      <c r="I116" s="26"/>
+    <row r="116" spans="1:9" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="25"/>
+      <c r="B116" s="25"/>
+      <c r="C116" s="25"/>
+      <c r="D116" s="22"/>
+      <c r="E116" s="22"/>
+      <c r="F116" s="22"/>
+      <c r="G116" s="22"/>
+      <c r="H116" s="22"/>
+      <c r="I116" s="25"/>
     </row>
     <row r="117" spans="1:9" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="36"/>
+      <c r="A117" s="26"/>
       <c r="B117" s="20"/>
-      <c r="C117" s="36"/>
-      <c r="D117" s="34"/>
-      <c r="E117" s="34"/>
-      <c r="F117" s="34"/>
-      <c r="G117" s="34"/>
-      <c r="H117" s="34"/>
-      <c r="I117" s="36"/>
-    </row>
-    <row r="118" spans="1:9" ht="12" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="C117" s="26"/>
+      <c r="D117" s="23"/>
+      <c r="E117" s="23"/>
+      <c r="F117" s="23"/>
+      <c r="G117" s="23"/>
+      <c r="H117" s="23"/>
+      <c r="I117" s="26"/>
+    </row>
+    <row r="118" spans="1:9" ht="12.75" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="F115:F117"/>
-    <mergeCell ref="G115:G117"/>
-    <mergeCell ref="H115:H117"/>
-    <mergeCell ref="I115:I117"/>
-    <mergeCell ref="A115:A117"/>
-    <mergeCell ref="B115:B116"/>
-    <mergeCell ref="C115:C117"/>
-    <mergeCell ref="D115:D117"/>
-    <mergeCell ref="E115:E117"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="A71:A74"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A51:A54"/>
-    <mergeCell ref="A55:A56"/>
     <mergeCell ref="A105:A108"/>
     <mergeCell ref="A109:A112"/>
     <mergeCell ref="B16:B17"/>
@@ -4231,6 +4199,38 @@
     <mergeCell ref="A85:A86"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A51:A54"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F115:F117"/>
+    <mergeCell ref="G115:G117"/>
+    <mergeCell ref="H115:H117"/>
+    <mergeCell ref="I115:I117"/>
+    <mergeCell ref="A115:A117"/>
+    <mergeCell ref="B115:B116"/>
+    <mergeCell ref="C115:C117"/>
+    <mergeCell ref="D115:D117"/>
+    <mergeCell ref="E115:E117"/>
   </mergeCells>
   <pageMargins left="0.94488188976377963" right="0.43307086614173229" top="1.5748031496062993" bottom="0.78740157480314965" header="0.39370078740157483" footer="0.15748031496062992"/>
   <pageSetup paperSize="9" scale="99" orientation="landscape" r:id="rId1"/>
@@ -4280,7 +4280,7 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -4343,56 +4343,31 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="0d2b025e-115d-408a-a85a-b3c0b0555798">YFMCKRR2ANA4-934254729-3851</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="0d2b025e-115d-408a-a85a-b3c0b0555798">
+      <Url>https://snsf.sharepoint.com/sites/IICT2/_layouts/15/DocIdRedir.aspx?ID=YFMCKRR2ANA4-934254729-3851</Url>
+      <Description>YFMCKRR2ANA4-934254729-3851</Description>
+    </_dlc_DocIdUrl>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9848c17d-c4de-492e-aed9-28e1e1dd577c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0d2b025e-115d-408a-a85a-b3c0b0555798" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101000B2CED907AAB97419F5CC195DD181113" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="96a1a0341db9437d5812900a4ced4744">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9848c17d-c4de-492e-aed9-28e1e1dd577c" xmlns:ns3="0d2b025e-115d-408a-a85a-b3c0b0555798" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="136d96f034136f668c87e1004ba5aa1f" ns2:_="" ns3:_="">
     <xsd:import namespace="9848c17d-c4de-492e-aed9-28e1e1dd577c"/>
@@ -4640,40 +4615,82 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="0d2b025e-115d-408a-a85a-b3c0b0555798">YFMCKRR2ANA4-934254729-3851</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="0d2b025e-115d-408a-a85a-b3c0b0555798">
-      <Url>https://snsf.sharepoint.com/sites/IICT2/_layouts/15/DocIdRedir.aspx?ID=YFMCKRR2ANA4-934254729-3851</Url>
-      <Description>YFMCKRR2ANA4-934254729-3851</Description>
-    </_dlc_DocIdUrl>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9848c17d-c4de-492e-aed9-28e1e1dd577c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0d2b025e-115d-408a-a85a-b3c0b0555798" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{486398B5-83E0-4D77-A37F-80A413420F70}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD528BF1-BC12-485A-AB0D-6E4CADEE8A83}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9848c17d-c4de-492e-aed9-28e1e1dd577c"/>
+    <ds:schemaRef ds:uri="0d2b025e-115d-408a-a85a-b3c0b0555798"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDE1ECD8-DB70-4A1D-B80E-CD4950BBB2F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{918B4902-D381-4BBA-9A1C-E6DC88A245B0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4692,27 +4709,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDE1ECD8-DB70-4A1D-B80E-CD4950BBB2F7}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{486398B5-83E0-4D77-A37F-80A413420F70}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD528BF1-BC12-485A-AB0D-6E4CADEE8A83}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9848c17d-c4de-492e-aed9-28e1e1dd577c"/>
-    <ds:schemaRef ds:uri="0d2b025e-115d-408a-a85a-b3c0b0555798"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>